<commit_message>
added summary assessment selectivity per specie
</commit_message>
<xml_diff>
--- a/time-varying/SpeciesBlock4kelli.xlsx
+++ b/time-varying/SpeciesBlock4kelli.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudio\Documents\SAFS_UW\Others\ICES_WG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudio\Documents\SAFS_UW\Others\ICES_WG\wg_MGWG\time-varying\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2167704-6AAE-4B3C-9D57-6639579907F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7BD81C6-E612-452B-AC78-8730E161770F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7788" windowHeight="5688" xr2:uid="{71844522-2DCB-46C4-9E69-8227D997BF2C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7500" windowHeight="5688" xr2:uid="{71844522-2DCB-46C4-9E69-8227D997BF2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>NSCod</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>USPollock and UStlHerring have two fleets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selectivity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management </t>
+  </si>
+  <si>
+    <t>Residuals</t>
   </si>
 </sst>
 </file>
@@ -537,19 +546,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BE33EA-13FB-45D6-B148-4D0FDC147B68}">
-  <dimension ref="B1:F36"/>
+  <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>5</v>
       </c>
@@ -563,10 +573,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -582,8 +598,14 @@
       <c r="F2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>2000</v>
+      </c>
+      <c r="H2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -600,7 +622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -617,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
@@ -634,7 +656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -651,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -668,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -685,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
@@ -702,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -719,7 +741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
@@ -736,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -753,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
@@ -770,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -787,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
@@ -804,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
@@ -1091,6 +1113,11 @@
       </c>
       <c r="F32" s="9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>